<commit_message>
clone onference issue fixed
</commit_message>
<xml_diff>
--- a/Individual Documents/Rudhra/PROJ_NAL11358736_CONSTRUCTION_2/Project Management/Task List -Iteration 3 - Epworth Project .xlsx
+++ b/Individual Documents/Rudhra/PROJ_NAL11358736_CONSTRUCTION_2/Project Management/Task List -Iteration 3 - Epworth Project .xlsx
@@ -2901,6 +2901,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6734175</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3539,6 +3587,54 @@
           <a:ahLst/>
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6848475</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 9"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
@@ -4211,6 +4307,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6867525</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4849,6 +4993,54 @@
           <a:ahLst/>
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
@@ -5521,6 +5713,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10002,8 +10242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>